<commit_message>
Added navigation bar option to add ingr that were logged as extra ingr in last logging with their logged amount and unit
</commit_message>
<xml_diff>
--- a/Excel_files/Log/Grocery_List_Log.xlsx
+++ b/Excel_files/Log/Grocery_List_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elskn\Projects\Grocery_list\Excel_files\Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF7BA75-5CC4-499D-A9CE-7A0EDEBA8444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8ABF67-0920-40C3-8C1D-2B1C86F3937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log Per Recipe" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="133">
   <si>
     <t>Recipe</t>
   </si>
@@ -320,16 +320,10 @@
     <t>Yoghurt Esh</t>
   </si>
   <si>
-    <t>Bananen</t>
-  </si>
-  <si>
     <t>Azijn</t>
   </si>
   <si>
     <t>Soya Melk</t>
-  </si>
-  <si>
-    <t>Appels</t>
   </si>
   <si>
     <t>Ananas</t>
@@ -487,14 +481,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -799,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
@@ -1616,22 +1608,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E36">
         <v>2.25</v>
       </c>
       <c r="F36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G36" s="2">
         <v>45783</v>
@@ -1639,7 +1631,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37">
         <v>9</v>
@@ -1662,16 +1654,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E38">
         <v>450</v>
@@ -1685,7 +1677,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -1708,7 +1700,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B40">
         <v>9</v>
@@ -1723,7 +1715,7 @@
         <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G40" s="2">
         <v>45783</v>
@@ -1731,7 +1723,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B41">
         <v>9</v>
@@ -1746,7 +1738,7 @@
         <v>2.25</v>
       </c>
       <c r="F41" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G41" s="2">
         <v>45783</v>
@@ -1754,7 +1746,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B42">
         <v>9</v>
@@ -1769,7 +1761,7 @@
         <v>2.25</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G42" s="2">
         <v>45783</v>
@@ -1777,16 +1769,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B43">
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E43">
         <v>90</v>
@@ -1800,7 +1792,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B44">
         <v>9</v>
@@ -1815,7 +1807,7 @@
         <v>2.25</v>
       </c>
       <c r="F44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G44" s="2">
         <v>45783</v>
@@ -1823,16 +1815,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E45">
         <v>9</v>
@@ -1846,22 +1838,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D46" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E46">
         <v>0.75</v>
       </c>
       <c r="F46" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G46" s="2">
         <v>45783</v>
@@ -1869,7 +1861,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -1892,16 +1884,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E48">
         <v>150</v>
@@ -1915,7 +1907,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -1938,7 +1930,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -1953,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G50" s="2">
         <v>45783</v>
@@ -1961,7 +1953,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -1976,7 +1968,7 @@
         <v>0.75</v>
       </c>
       <c r="F51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G51" s="2">
         <v>45783</v>
@@ -1984,7 +1976,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -1999,7 +1991,7 @@
         <v>0.75</v>
       </c>
       <c r="F52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G52" s="2">
         <v>45783</v>
@@ -2007,16 +1999,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E53">
         <v>30</v>
@@ -2030,7 +2022,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -2045,7 +2037,7 @@
         <v>0.75</v>
       </c>
       <c r="F54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G54" s="2">
         <v>45783</v>
@@ -2237,7 +2229,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -2260,16 +2252,16 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B64">
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D64" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E64">
         <v>32</v>
@@ -2283,7 +2275,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B65">
         <v>4</v>
@@ -2292,7 +2284,7 @@
         <v>94</v>
       </c>
       <c r="D65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -2306,16 +2298,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B66">
         <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E66">
         <v>8</v>
@@ -2329,16 +2321,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B67">
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E67">
         <v>8</v>
@@ -2352,16 +2344,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B68">
         <v>4</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E68">
         <v>80</v>
@@ -2375,16 +2367,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E69">
         <v>1.32</v>
@@ -2398,7 +2390,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -2407,7 +2399,7 @@
         <v>95</v>
       </c>
       <c r="D70" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E70">
         <v>500</v>
@@ -2904,7 +2896,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B92">
         <v>3</v>
@@ -2927,7 +2919,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B93">
         <v>3</v>
@@ -2950,7 +2942,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -2973,7 +2965,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -2996,7 +2988,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -3019,7 +3011,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -3042,7 +3034,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -3065,7 +3057,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -3088,7 +3080,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B100">
         <v>3</v>
@@ -3111,7 +3103,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -3134,7 +3126,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -3157,7 +3149,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -3180,7 +3172,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -3203,7 +3195,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -3226,7 +3218,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -3249,7 +3241,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B107">
         <v>3</v>
@@ -3272,7 +3264,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -3295,7 +3287,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B109">
         <v>3</v>
@@ -3318,7 +3310,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -3341,7 +3333,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -3364,7 +3356,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -3387,7 +3379,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -3410,7 +3402,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -3433,7 +3425,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -3456,7 +3448,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -3478,22 +3470,22 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="4" t="s">
+      <c r="A117" t="s">
         <v>7</v>
       </c>
-      <c r="B117" s="4">
+      <c r="B117">
         <v>7</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C117" t="s">
         <v>8</v>
       </c>
-      <c r="D117" s="4" t="s">
+      <c r="D117" t="s">
         <v>9</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117">
         <v>1225</v>
       </c>
-      <c r="F117" s="4" t="s">
+      <c r="F117" t="s">
         <v>10</v>
       </c>
       <c r="G117" s="2">
@@ -3501,22 +3493,22 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="4" t="s">
+      <c r="A118" t="s">
         <v>7</v>
       </c>
-      <c r="B118" s="4">
+      <c r="B118">
         <v>7</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" t="s">
         <v>11</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" t="s">
         <v>12</v>
       </c>
-      <c r="E118" s="4">
+      <c r="E118">
         <v>1400</v>
       </c>
-      <c r="F118" s="4" t="s">
+      <c r="F118" t="s">
         <v>10</v>
       </c>
       <c r="G118" s="2">
@@ -3524,22 +3516,22 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="4" t="s">
+      <c r="A119" t="s">
         <v>7</v>
       </c>
-      <c r="B119" s="4">
+      <c r="B119">
         <v>7</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="C119" t="s">
         <v>13</v>
       </c>
-      <c r="D119" s="4" t="s">
+      <c r="D119" t="s">
         <v>14</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119">
         <v>7</v>
       </c>
-      <c r="F119" s="4" t="s">
+      <c r="F119" t="s">
         <v>15</v>
       </c>
       <c r="G119" s="2">
@@ -3547,22 +3539,22 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="4" t="s">
+      <c r="A120" t="s">
         <v>7</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B120">
         <v>7</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" t="s">
         <v>16</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" t="s">
         <v>17</v>
       </c>
-      <c r="E120" s="4">
+      <c r="E120">
         <v>420</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="F120" t="s">
         <v>10</v>
       </c>
       <c r="G120" s="2">
@@ -3570,22 +3562,22 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="4" t="s">
+      <c r="A121" t="s">
         <v>7</v>
       </c>
-      <c r="B121" s="4">
+      <c r="B121">
         <v>7</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" t="s">
         <v>18</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" t="s">
         <v>19</v>
       </c>
-      <c r="E121" s="4">
+      <c r="E121">
         <v>7</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="F121" t="s">
         <v>15</v>
       </c>
       <c r="G121" s="2">
@@ -3593,22 +3585,22 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="4" t="s">
+      <c r="A122" t="s">
         <v>7</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B122">
         <v>7</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" t="s">
         <v>20</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D122" t="s">
         <v>21</v>
       </c>
-      <c r="E122" s="4">
+      <c r="E122">
         <v>161</v>
       </c>
-      <c r="F122" s="4" t="s">
+      <c r="F122" t="s">
         <v>10</v>
       </c>
       <c r="G122" s="2">
@@ -3616,22 +3608,22 @@
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="4" t="s">
+      <c r="A123" t="s">
         <v>7</v>
       </c>
-      <c r="B123" s="4">
+      <c r="B123">
         <v>7</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C123" t="s">
         <v>22</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D123" t="s">
         <v>23</v>
       </c>
-      <c r="E123" s="4">
+      <c r="E123">
         <v>154</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F123" t="s">
         <v>10</v>
       </c>
       <c r="G123" s="2">
@@ -3639,22 +3631,22 @@
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B124" s="4">
+      <c r="A124" t="s">
+        <v>122</v>
+      </c>
+      <c r="B124">
         <v>4</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C124" t="s">
         <v>53</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D124" t="s">
         <v>54</v>
       </c>
-      <c r="E124" s="4">
+      <c r="E124">
         <v>4</v>
       </c>
-      <c r="F124" s="4" t="s">
+      <c r="F124" t="s">
         <v>15</v>
       </c>
       <c r="G124" s="2">
@@ -3662,22 +3654,22 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B125" s="4">
+      <c r="A125" t="s">
+        <v>122</v>
+      </c>
+      <c r="B125">
         <v>4</v>
       </c>
-      <c r="C125" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E125" s="4">
+      <c r="C125" t="s">
+        <v>111</v>
+      </c>
+      <c r="D125" t="s">
+        <v>123</v>
+      </c>
+      <c r="E125">
         <v>32</v>
       </c>
-      <c r="F125" s="4" t="s">
+      <c r="F125" t="s">
         <v>10</v>
       </c>
       <c r="G125" s="2">
@@ -3685,22 +3677,22 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="4" t="s">
+      <c r="A126" t="s">
+        <v>122</v>
+      </c>
+      <c r="B126">
+        <v>4</v>
+      </c>
+      <c r="C126" t="s">
+        <v>94</v>
+      </c>
+      <c r="D126" t="s">
         <v>124</v>
       </c>
-      <c r="B126" s="4">
-        <v>4</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E126" s="4">
+      <c r="E126">
         <v>2</v>
       </c>
-      <c r="F126" s="4" t="s">
+      <c r="F126" t="s">
         <v>15</v>
       </c>
       <c r="G126" s="2">
@@ -3708,22 +3700,22 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B127" s="4">
+      <c r="A127" t="s">
+        <v>122</v>
+      </c>
+      <c r="B127">
         <v>4</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D127" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E127" s="4">
+      <c r="C127" t="s">
+        <v>104</v>
+      </c>
+      <c r="D127" t="s">
+        <v>125</v>
+      </c>
+      <c r="E127">
         <v>8</v>
       </c>
-      <c r="F127" s="4" t="s">
+      <c r="F127" t="s">
         <v>10</v>
       </c>
       <c r="G127" s="2">
@@ -3731,22 +3723,22 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B128" s="4">
+      <c r="A128" t="s">
+        <v>122</v>
+      </c>
+      <c r="B128">
         <v>4</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E128" s="4">
+      <c r="C128" t="s">
+        <v>113</v>
+      </c>
+      <c r="D128" t="s">
+        <v>126</v>
+      </c>
+      <c r="E128">
         <v>8</v>
       </c>
-      <c r="F128" s="4" t="s">
+      <c r="F128" t="s">
         <v>10</v>
       </c>
       <c r="G128" s="2">
@@ -3754,22 +3746,22 @@
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B129" s="4">
+      <c r="A129" t="s">
+        <v>122</v>
+      </c>
+      <c r="B129">
         <v>4</v>
       </c>
-      <c r="C129" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E129" s="4">
-        <v>80</v>
-      </c>
-      <c r="F129" s="4" t="s">
+      <c r="C129" t="s">
+        <v>107</v>
+      </c>
+      <c r="D129" t="s">
+        <v>127</v>
+      </c>
+      <c r="E129">
+        <v>80</v>
+      </c>
+      <c r="F129" t="s">
         <v>10</v>
       </c>
       <c r="G129" s="2">
@@ -3777,22 +3769,22 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B130" s="4">
+      <c r="A130" t="s">
+        <v>122</v>
+      </c>
+      <c r="B130">
         <v>4</v>
       </c>
-      <c r="C130" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E130" s="4">
+      <c r="C130" t="s">
+        <v>105</v>
+      </c>
+      <c r="D130" t="s">
+        <v>128</v>
+      </c>
+      <c r="E130">
         <v>1.32</v>
       </c>
-      <c r="F130" s="4" t="s">
+      <c r="F130" t="s">
         <v>15</v>
       </c>
       <c r="G130" s="2">
@@ -3800,22 +3792,22 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B131" s="4">
+      <c r="A131" t="s">
+        <v>122</v>
+      </c>
+      <c r="B131">
         <v>4</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" t="s">
         <v>95</v>
       </c>
-      <c r="D131" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E131" s="4">
+      <c r="D131" t="s">
+        <v>129</v>
+      </c>
+      <c r="E131">
         <v>500</v>
       </c>
-      <c r="F131" s="4" t="s">
+      <c r="F131" t="s">
         <v>10</v>
       </c>
       <c r="G131" s="2">
@@ -3823,22 +3815,22 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="4" t="s">
+      <c r="A132" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="4">
+      <c r="B132">
         <v>6</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" t="s">
         <v>58</v>
       </c>
-      <c r="D132" s="4" t="s">
+      <c r="D132" t="s">
         <v>59</v>
       </c>
-      <c r="E132" s="4">
+      <c r="E132">
         <v>1</v>
       </c>
-      <c r="F132" s="4" t="s">
+      <c r="F132" t="s">
         <v>15</v>
       </c>
       <c r="G132" s="2">
@@ -3846,22 +3838,22 @@
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="4" t="s">
+      <c r="A133" t="s">
         <v>57</v>
       </c>
-      <c r="B133" s="4">
+      <c r="B133">
         <v>6</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C133" t="s">
         <v>60</v>
       </c>
-      <c r="D133" s="4" t="s">
+      <c r="D133" t="s">
         <v>61</v>
       </c>
-      <c r="E133" s="4">
+      <c r="E133">
         <v>234</v>
       </c>
-      <c r="F133" s="4" t="s">
+      <c r="F133" t="s">
         <v>10</v>
       </c>
       <c r="G133" s="2">
@@ -3869,22 +3861,22 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="4" t="s">
+      <c r="A134" t="s">
         <v>57</v>
       </c>
-      <c r="B134" s="4">
+      <c r="B134">
         <v>6</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" t="s">
         <v>62</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="D134" t="s">
         <v>63</v>
       </c>
-      <c r="E134" s="4">
+      <c r="E134">
         <v>150</v>
       </c>
-      <c r="F134" s="4" t="s">
+      <c r="F134" t="s">
         <v>10</v>
       </c>
       <c r="G134" s="2">
@@ -3892,22 +3884,22 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="4" t="s">
+      <c r="A135" t="s">
         <v>57</v>
       </c>
-      <c r="B135" s="4">
+      <c r="B135">
         <v>6</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" t="s">
         <v>64</v>
       </c>
-      <c r="D135" s="4" t="s">
+      <c r="D135" t="s">
         <v>65</v>
       </c>
-      <c r="E135" s="4">
+      <c r="E135">
         <v>90</v>
       </c>
-      <c r="F135" s="4" t="s">
+      <c r="F135" t="s">
         <v>10</v>
       </c>
       <c r="G135" s="2">
@@ -3915,22 +3907,22 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="4" t="s">
+      <c r="A136" t="s">
         <v>57</v>
       </c>
-      <c r="B136" s="4">
+      <c r="B136">
         <v>6</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" t="s">
         <v>53</v>
       </c>
-      <c r="D136" s="4" t="s">
+      <c r="D136" t="s">
         <v>54</v>
       </c>
-      <c r="E136" s="4">
+      <c r="E136">
         <v>4.8000000000000007</v>
       </c>
-      <c r="F136" s="4" t="s">
+      <c r="F136" t="s">
         <v>15</v>
       </c>
       <c r="G136" s="2">
@@ -3938,22 +3930,22 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="4" t="s">
+      <c r="A137" t="s">
         <v>57</v>
       </c>
-      <c r="B137" s="4">
+      <c r="B137">
         <v>6</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C137" t="s">
         <v>35</v>
       </c>
-      <c r="D137" s="4" t="s">
+      <c r="D137" t="s">
         <v>36</v>
       </c>
-      <c r="E137" s="4">
+      <c r="E137">
         <v>150</v>
       </c>
-      <c r="F137" s="4" t="s">
+      <c r="F137" t="s">
         <v>10</v>
       </c>
       <c r="G137" s="2">
@@ -3961,22 +3953,22 @@
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="4" t="s">
+      <c r="A138" t="s">
         <v>57</v>
       </c>
-      <c r="B138" s="4">
+      <c r="B138">
         <v>6</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" t="s">
         <v>66</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D138" t="s">
         <v>67</v>
       </c>
-      <c r="E138" s="4">
+      <c r="E138">
         <v>90</v>
       </c>
-      <c r="F138" s="4" t="s">
+      <c r="F138" t="s">
         <v>10</v>
       </c>
       <c r="G138" s="2">
@@ -3984,22 +3976,22 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="4" t="s">
+      <c r="A139" t="s">
         <v>57</v>
       </c>
-      <c r="B139" s="4">
+      <c r="B139">
         <v>6</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C139" t="s">
         <v>68</v>
       </c>
-      <c r="D139" s="4" t="s">
+      <c r="D139" t="s">
         <v>69</v>
       </c>
-      <c r="E139" s="4">
+      <c r="E139">
         <v>300</v>
       </c>
-      <c r="F139" s="4" t="s">
+      <c r="F139" t="s">
         <v>10</v>
       </c>
       <c r="G139" s="2">
@@ -4015,12 +4007,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="14.68359375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.41796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4432,7 +4425,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -4446,7 +4439,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4516,7 +4509,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -4572,7 +4565,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4586,7 +4579,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4600,7 +4593,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B42">
         <v>20</v>
@@ -4628,7 +4621,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -4642,7 +4635,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B45">
         <v>8</v>
@@ -4810,7 +4803,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B57">
         <v>1.32</v>
@@ -4894,7 +4887,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63">
         <v>10</v>
@@ -5020,7 +5013,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B72">
         <v>80</v>
@@ -5076,7 +5069,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B76">
         <v>120</v>
@@ -5146,7 +5139,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -5174,7 +5167,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B83">
         <v>600</v>
@@ -5230,7 +5223,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B87">
         <v>32</v>
@@ -5272,7 +5265,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B90">
         <v>9</v>
@@ -5286,7 +5279,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B91">
         <v>8</v>
@@ -5299,13 +5292,13 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B92" s="3">
+      <c r="A92" t="s">
+        <v>132</v>
+      </c>
+      <c r="B92">
         <v>1</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" t="s">
         <v>15</v>
       </c>
       <c r="D92" s="2">
@@ -5313,13 +5306,13 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B93" s="3">
+      <c r="A93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93">
         <v>1</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" t="s">
         <v>15</v>
       </c>
       <c r="D93" s="2">
@@ -5327,13 +5320,13 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B94" s="3">
+      <c r="A94" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94">
         <v>18</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" t="s">
         <v>15</v>
       </c>
       <c r="D94" s="2">
@@ -5341,13 +5334,13 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B95" s="3">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95">
         <v>8</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="2">
@@ -5355,13 +5348,13 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="3" t="s">
+      <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96">
         <v>3</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C96" t="s">
         <v>15</v>
       </c>
       <c r="D96" s="2">
@@ -5369,13 +5362,13 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="3" t="s">
+      <c r="A97" t="s">
         <v>58</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97">
         <v>1</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" t="s">
         <v>15</v>
       </c>
       <c r="D97" s="2">
@@ -5383,13 +5376,13 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="3" t="s">
+      <c r="A98" t="s">
         <v>11</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98">
         <v>1400</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" t="s">
         <v>10</v>
       </c>
       <c r="D98" s="2">
@@ -5397,13 +5390,13 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="3" t="s">
+      <c r="A99" t="s">
         <v>35</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99">
         <v>150</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" t="s">
         <v>10</v>
       </c>
       <c r="D99" s="2">
@@ -5411,13 +5404,13 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="3" t="s">
+      <c r="A100" t="s">
         <v>95</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100">
         <v>500</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" t="s">
         <v>10</v>
       </c>
       <c r="D100" s="2">
@@ -5425,13 +5418,13 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="3" t="s">
+      <c r="A101" t="s">
         <v>95</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101">
         <v>2</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" t="s">
         <v>15</v>
       </c>
       <c r="D101" s="2">
@@ -5439,13 +5432,13 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="3" t="s">
+      <c r="A102" t="s">
         <v>43</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102">
         <v>1050</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C102" t="s">
         <v>10</v>
       </c>
       <c r="D102" s="2">
@@ -5453,13 +5446,13 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="3" t="s">
+      <c r="A103" t="s">
         <v>53</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103">
         <v>54.8</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C103" t="s">
         <v>15</v>
       </c>
       <c r="D103" s="2">
@@ -5467,13 +5460,13 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B104" s="3">
+      <c r="A104" t="s">
+        <v>105</v>
+      </c>
+      <c r="B104">
         <v>1.32</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C104" t="s">
         <v>15</v>
       </c>
       <c r="D104" s="2">
@@ -5481,13 +5474,13 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="3" t="s">
+      <c r="A105" t="s">
         <v>18</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105">
         <v>7</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="C105" t="s">
         <v>15</v>
       </c>
       <c r="D105" s="2">
@@ -5495,13 +5488,13 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="3" t="s">
+      <c r="A106" t="s">
         <v>13</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106">
         <v>7</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C106" t="s">
         <v>15</v>
       </c>
       <c r="D106" s="2">
@@ -5509,13 +5502,13 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="3" t="s">
+      <c r="A107" t="s">
         <v>55</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107">
         <v>1</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C107" t="s">
         <v>15</v>
       </c>
       <c r="D107" s="2">
@@ -5523,13 +5516,13 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="3" t="s">
+      <c r="A108" t="s">
         <v>22</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108">
         <v>154</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" t="s">
         <v>10</v>
       </c>
       <c r="D108" s="2">
@@ -5537,13 +5530,13 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="3" t="s">
+      <c r="A109" t="s">
         <v>66</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109">
         <v>90</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="C109" t="s">
         <v>10</v>
       </c>
       <c r="D109" s="2">
@@ -5551,13 +5544,13 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="3" t="s">
+      <c r="A110" t="s">
         <v>64</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110">
         <v>90</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" t="s">
         <v>10</v>
       </c>
       <c r="D110" s="2">
@@ -5565,13 +5558,13 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="3" t="s">
+      <c r="A111" t="s">
         <v>60</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111">
         <v>234</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" t="s">
         <v>10</v>
       </c>
       <c r="D111" s="2">
@@ -5579,13 +5572,13 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B112" s="3">
-        <v>80</v>
-      </c>
-      <c r="C112" s="3" t="s">
+      <c r="A112" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112">
+        <v>80</v>
+      </c>
+      <c r="C112" t="s">
         <v>10</v>
       </c>
       <c r="D112" s="2">
@@ -5593,13 +5586,13 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="3" t="s">
+      <c r="A113" t="s">
         <v>16</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113">
         <v>420</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" t="s">
         <v>10</v>
       </c>
       <c r="D113" s="2">
@@ -5607,13 +5600,13 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="3" t="s">
+      <c r="A114" t="s">
         <v>68</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114">
         <v>300</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" t="s">
         <v>10</v>
       </c>
       <c r="D114" s="2">
@@ -5621,13 +5614,13 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="3" t="s">
+      <c r="A115" t="s">
         <v>96</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115">
         <v>1</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" t="s">
         <v>15</v>
       </c>
       <c r="D115" s="2">
@@ -5635,13 +5628,13 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="3" t="s">
+      <c r="A116" t="s">
         <v>20</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B116">
         <v>161</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" t="s">
         <v>10</v>
       </c>
       <c r="D116" s="2">
@@ -5649,13 +5642,13 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="3" t="s">
+      <c r="A117" t="s">
         <v>8</v>
       </c>
-      <c r="B117" s="3">
+      <c r="B117">
         <v>1225</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C117" t="s">
         <v>10</v>
       </c>
       <c r="D117" s="2">
@@ -5663,13 +5656,13 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B118" s="3">
+      <c r="A118" t="s">
+        <v>111</v>
+      </c>
+      <c r="B118">
         <v>32</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C118" t="s">
         <v>10</v>
       </c>
       <c r="D118" s="2">
@@ -5677,13 +5670,13 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="3" t="s">
+      <c r="A119" t="s">
         <v>97</v>
       </c>
-      <c r="B119" s="3">
+      <c r="B119">
         <v>1</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" t="s">
         <v>15</v>
       </c>
       <c r="D119" s="2">
@@ -5691,13 +5684,13 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="3" t="s">
+      <c r="A120" t="s">
         <v>62</v>
       </c>
-      <c r="B120" s="3">
+      <c r="B120">
         <v>150</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" t="s">
         <v>10</v>
       </c>
       <c r="D120" s="2">
@@ -5705,13 +5698,13 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B121" s="3">
+      <c r="A121" t="s">
+        <v>113</v>
+      </c>
+      <c r="B121">
         <v>8</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" t="s">
         <v>10</v>
       </c>
       <c r="D121" s="2">

</xml_diff>

<commit_message>
Export Groceris 2 - 06
</commit_message>
<xml_diff>
--- a/Excel_files/Log/Grocery_List_Log.xlsx
+++ b/Excel_files/Log/Grocery_List_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elskn\Projects\Grocery_list\Excel_files\Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC9CF77-8BC5-4323-9268-C6777FD4F920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AD2461-6270-42C4-A20A-55CE7FA0FA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="504" windowWidth="12498" windowHeight="11802" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log Per Recipe" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="143">
   <si>
     <t>Recipe</t>
   </si>
@@ -441,6 +441,15 @@
   </si>
   <si>
     <t>SUPERGEHAKT</t>
+  </si>
+  <si>
+    <t>Pindakaas</t>
+  </si>
+  <si>
+    <t>Granaatappel</t>
+  </si>
+  <si>
+    <t>Peer</t>
   </si>
 </sst>
 </file>
@@ -810,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G176"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="G173" sqref="G173"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="G197" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4870,6 +4879,558 @@
         <v>45803</v>
       </c>
     </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177">
+        <v>11</v>
+      </c>
+      <c r="C177" t="s">
+        <v>8</v>
+      </c>
+      <c r="D177" t="s">
+        <v>9</v>
+      </c>
+      <c r="E177">
+        <v>1925</v>
+      </c>
+      <c r="F177" t="s">
+        <v>10</v>
+      </c>
+      <c r="G177" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" t="s">
+        <v>7</v>
+      </c>
+      <c r="B178">
+        <v>11</v>
+      </c>
+      <c r="C178" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" t="s">
+        <v>12</v>
+      </c>
+      <c r="E178">
+        <v>2200</v>
+      </c>
+      <c r="F178" t="s">
+        <v>10</v>
+      </c>
+      <c r="G178" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" t="s">
+        <v>7</v>
+      </c>
+      <c r="B179">
+        <v>11</v>
+      </c>
+      <c r="C179" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" t="s">
+        <v>14</v>
+      </c>
+      <c r="E179">
+        <v>11</v>
+      </c>
+      <c r="F179" t="s">
+        <v>15</v>
+      </c>
+      <c r="G179" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" t="s">
+        <v>7</v>
+      </c>
+      <c r="B180">
+        <v>11</v>
+      </c>
+      <c r="C180" t="s">
+        <v>16</v>
+      </c>
+      <c r="D180" t="s">
+        <v>17</v>
+      </c>
+      <c r="E180">
+        <v>660</v>
+      </c>
+      <c r="F180" t="s">
+        <v>10</v>
+      </c>
+      <c r="G180" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" t="s">
+        <v>7</v>
+      </c>
+      <c r="B181">
+        <v>11</v>
+      </c>
+      <c r="C181" t="s">
+        <v>18</v>
+      </c>
+      <c r="D181" t="s">
+        <v>19</v>
+      </c>
+      <c r="E181">
+        <v>11</v>
+      </c>
+      <c r="F181" t="s">
+        <v>15</v>
+      </c>
+      <c r="G181" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" t="s">
+        <v>7</v>
+      </c>
+      <c r="B182">
+        <v>11</v>
+      </c>
+      <c r="C182" t="s">
+        <v>20</v>
+      </c>
+      <c r="D182" t="s">
+        <v>21</v>
+      </c>
+      <c r="E182">
+        <v>253</v>
+      </c>
+      <c r="F182" t="s">
+        <v>10</v>
+      </c>
+      <c r="G182" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" t="s">
+        <v>7</v>
+      </c>
+      <c r="B183">
+        <v>11</v>
+      </c>
+      <c r="C183" t="s">
+        <v>22</v>
+      </c>
+      <c r="D183" t="s">
+        <v>23</v>
+      </c>
+      <c r="E183">
+        <v>242</v>
+      </c>
+      <c r="F183" t="s">
+        <v>10</v>
+      </c>
+      <c r="G183" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" t="s">
+        <v>81</v>
+      </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
+      <c r="C184" t="s">
+        <v>82</v>
+      </c>
+      <c r="D184" t="s">
+        <v>83</v>
+      </c>
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184" t="s">
+        <v>15</v>
+      </c>
+      <c r="G184" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" t="s">
+        <v>81</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>84</v>
+      </c>
+      <c r="D185" t="s">
+        <v>85</v>
+      </c>
+      <c r="E185">
+        <v>75</v>
+      </c>
+      <c r="F185" t="s">
+        <v>10</v>
+      </c>
+      <c r="G185" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" t="s">
+        <v>81</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="C186" t="s">
+        <v>64</v>
+      </c>
+      <c r="D186" t="s">
+        <v>65</v>
+      </c>
+      <c r="E186">
+        <v>50</v>
+      </c>
+      <c r="F186" t="s">
+        <v>10</v>
+      </c>
+      <c r="G186" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" t="s">
+        <v>86</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187" t="s">
+        <v>82</v>
+      </c>
+      <c r="D187" t="s">
+        <v>83</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>15</v>
+      </c>
+      <c r="G187" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" t="s">
+        <v>86</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188" t="s">
+        <v>84</v>
+      </c>
+      <c r="D188" t="s">
+        <v>85</v>
+      </c>
+      <c r="E188">
+        <v>75</v>
+      </c>
+      <c r="F188" t="s">
+        <v>10</v>
+      </c>
+      <c r="G188" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" t="s">
+        <v>86</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189" t="s">
+        <v>64</v>
+      </c>
+      <c r="D189" t="s">
+        <v>65</v>
+      </c>
+      <c r="E189">
+        <v>50</v>
+      </c>
+      <c r="F189" t="s">
+        <v>10</v>
+      </c>
+      <c r="G189" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" t="s">
+        <v>86</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+      <c r="C190" t="s">
+        <v>87</v>
+      </c>
+      <c r="D190" t="s">
+        <v>88</v>
+      </c>
+      <c r="E190">
+        <v>25</v>
+      </c>
+      <c r="F190" t="s">
+        <v>10</v>
+      </c>
+      <c r="G190" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" t="s">
+        <v>86</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191" t="s">
+        <v>24</v>
+      </c>
+      <c r="D191" t="s">
+        <v>25</v>
+      </c>
+      <c r="E191">
+        <v>1</v>
+      </c>
+      <c r="F191" t="s">
+        <v>15</v>
+      </c>
+      <c r="G191" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" t="s">
+        <v>86</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
+        <v>37</v>
+      </c>
+      <c r="D192" t="s">
+        <v>38</v>
+      </c>
+      <c r="E192">
+        <v>0.5</v>
+      </c>
+      <c r="F192" t="s">
+        <v>15</v>
+      </c>
+      <c r="G192" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" t="s">
+        <v>57</v>
+      </c>
+      <c r="B193">
+        <v>12</v>
+      </c>
+      <c r="C193" t="s">
+        <v>58</v>
+      </c>
+      <c r="D193" t="s">
+        <v>59</v>
+      </c>
+      <c r="E193">
+        <v>2</v>
+      </c>
+      <c r="F193" t="s">
+        <v>15</v>
+      </c>
+      <c r="G193" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" t="s">
+        <v>57</v>
+      </c>
+      <c r="B194">
+        <v>12</v>
+      </c>
+      <c r="C194" t="s">
+        <v>60</v>
+      </c>
+      <c r="D194" t="s">
+        <v>61</v>
+      </c>
+      <c r="E194">
+        <v>468</v>
+      </c>
+      <c r="F194" t="s">
+        <v>10</v>
+      </c>
+      <c r="G194" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" t="s">
+        <v>57</v>
+      </c>
+      <c r="B195">
+        <v>12</v>
+      </c>
+      <c r="C195" t="s">
+        <v>62</v>
+      </c>
+      <c r="D195" t="s">
+        <v>63</v>
+      </c>
+      <c r="E195">
+        <v>300</v>
+      </c>
+      <c r="F195" t="s">
+        <v>10</v>
+      </c>
+      <c r="G195" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" t="s">
+        <v>57</v>
+      </c>
+      <c r="B196">
+        <v>12</v>
+      </c>
+      <c r="C196" t="s">
+        <v>64</v>
+      </c>
+      <c r="D196" t="s">
+        <v>65</v>
+      </c>
+      <c r="E196">
+        <v>180</v>
+      </c>
+      <c r="F196" t="s">
+        <v>10</v>
+      </c>
+      <c r="G196" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" t="s">
+        <v>57</v>
+      </c>
+      <c r="B197">
+        <v>12</v>
+      </c>
+      <c r="C197" t="s">
+        <v>53</v>
+      </c>
+      <c r="D197" t="s">
+        <v>54</v>
+      </c>
+      <c r="E197">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="F197" t="s">
+        <v>15</v>
+      </c>
+      <c r="G197" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" t="s">
+        <v>57</v>
+      </c>
+      <c r="B198">
+        <v>12</v>
+      </c>
+      <c r="C198" t="s">
+        <v>35</v>
+      </c>
+      <c r="D198" t="s">
+        <v>36</v>
+      </c>
+      <c r="E198">
+        <v>300</v>
+      </c>
+      <c r="F198" t="s">
+        <v>10</v>
+      </c>
+      <c r="G198" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" t="s">
+        <v>57</v>
+      </c>
+      <c r="B199">
+        <v>12</v>
+      </c>
+      <c r="C199" t="s">
+        <v>66</v>
+      </c>
+      <c r="D199" t="s">
+        <v>67</v>
+      </c>
+      <c r="E199">
+        <v>180</v>
+      </c>
+      <c r="F199" t="s">
+        <v>10</v>
+      </c>
+      <c r="G199" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" t="s">
+        <v>57</v>
+      </c>
+      <c r="B200">
+        <v>12</v>
+      </c>
+      <c r="C200" t="s">
+        <v>68</v>
+      </c>
+      <c r="D200" t="s">
+        <v>69</v>
+      </c>
+      <c r="E200">
+        <v>600</v>
+      </c>
+      <c r="F200" t="s">
+        <v>10</v>
+      </c>
+      <c r="G200" s="2">
+        <v>45810</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4877,10 +5438,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7031,6 +7592,482 @@
         <v>45803</v>
       </c>
     </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" t="s">
+        <v>101</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" t="s">
+        <v>87</v>
+      </c>
+      <c r="B155">
+        <v>25</v>
+      </c>
+      <c r="C155" t="s">
+        <v>10</v>
+      </c>
+      <c r="D155" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" t="s">
+        <v>102</v>
+      </c>
+      <c r="B156">
+        <v>20</v>
+      </c>
+      <c r="C156" t="s">
+        <v>15</v>
+      </c>
+      <c r="D156" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" t="s">
+        <v>94</v>
+      </c>
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157" t="s">
+        <v>15</v>
+      </c>
+      <c r="D157" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" t="s">
+        <v>58</v>
+      </c>
+      <c r="B158">
+        <v>2</v>
+      </c>
+      <c r="C158" t="s">
+        <v>15</v>
+      </c>
+      <c r="D158" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" t="s">
+        <v>11</v>
+      </c>
+      <c r="B159">
+        <v>2200</v>
+      </c>
+      <c r="C159" t="s">
+        <v>10</v>
+      </c>
+      <c r="D159" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" t="s">
+        <v>35</v>
+      </c>
+      <c r="B160">
+        <v>300</v>
+      </c>
+      <c r="C160" t="s">
+        <v>10</v>
+      </c>
+      <c r="D160" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" t="s">
+        <v>37</v>
+      </c>
+      <c r="B161">
+        <v>0.5</v>
+      </c>
+      <c r="C161" t="s">
+        <v>15</v>
+      </c>
+      <c r="D161" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" t="s">
+        <v>95</v>
+      </c>
+      <c r="B162">
+        <v>2</v>
+      </c>
+      <c r="C162" t="s">
+        <v>15</v>
+      </c>
+      <c r="D162" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" t="s">
+        <v>43</v>
+      </c>
+      <c r="B163">
+        <v>1200</v>
+      </c>
+      <c r="C163" t="s">
+        <v>10</v>
+      </c>
+      <c r="D163" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" t="s">
+        <v>53</v>
+      </c>
+      <c r="B164">
+        <v>45.6</v>
+      </c>
+      <c r="C164" t="s">
+        <v>15</v>
+      </c>
+      <c r="D164" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" t="s">
+        <v>18</v>
+      </c>
+      <c r="B165">
+        <v>11</v>
+      </c>
+      <c r="C165" t="s">
+        <v>15</v>
+      </c>
+      <c r="D165" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" t="s">
+        <v>13</v>
+      </c>
+      <c r="B166">
+        <v>11</v>
+      </c>
+      <c r="C166" t="s">
+        <v>15</v>
+      </c>
+      <c r="D166" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" t="s">
+        <v>55</v>
+      </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
+      <c r="C167" t="s">
+        <v>15</v>
+      </c>
+      <c r="D167" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" t="s">
+        <v>22</v>
+      </c>
+      <c r="B168">
+        <v>242</v>
+      </c>
+      <c r="C168" t="s">
+        <v>10</v>
+      </c>
+      <c r="D168" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" t="s">
+        <v>66</v>
+      </c>
+      <c r="B169">
+        <v>180</v>
+      </c>
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+      <c r="D169" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" t="s">
+        <v>64</v>
+      </c>
+      <c r="B170">
+        <v>280</v>
+      </c>
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+      <c r="D170" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" t="s">
+        <v>84</v>
+      </c>
+      <c r="B171">
+        <v>150</v>
+      </c>
+      <c r="C171" t="s">
+        <v>10</v>
+      </c>
+      <c r="D171" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" t="s">
+        <v>140</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+      <c r="C172" t="s">
+        <v>15</v>
+      </c>
+      <c r="D172" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" t="s">
+        <v>82</v>
+      </c>
+      <c r="B173">
+        <v>2</v>
+      </c>
+      <c r="C173" t="s">
+        <v>15</v>
+      </c>
+      <c r="D173" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" t="s">
+        <v>60</v>
+      </c>
+      <c r="B174">
+        <v>468</v>
+      </c>
+      <c r="C174" t="s">
+        <v>10</v>
+      </c>
+      <c r="D174" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" t="s">
+        <v>16</v>
+      </c>
+      <c r="B175">
+        <v>660</v>
+      </c>
+      <c r="C175" t="s">
+        <v>10</v>
+      </c>
+      <c r="D175" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
+        <v>15</v>
+      </c>
+      <c r="D176" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" t="s">
+        <v>68</v>
+      </c>
+      <c r="B177">
+        <v>600</v>
+      </c>
+      <c r="C177" t="s">
+        <v>10</v>
+      </c>
+      <c r="D177" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" t="s">
+        <v>96</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178" t="s">
+        <v>15</v>
+      </c>
+      <c r="D178" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" t="s">
+        <v>109</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+      <c r="C179" t="s">
+        <v>15</v>
+      </c>
+      <c r="D179" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" t="s">
+        <v>20</v>
+      </c>
+      <c r="B180">
+        <v>253</v>
+      </c>
+      <c r="C180" t="s">
+        <v>10</v>
+      </c>
+      <c r="D180" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" t="s">
+        <v>8</v>
+      </c>
+      <c r="B181">
+        <v>1925</v>
+      </c>
+      <c r="C181" t="s">
+        <v>10</v>
+      </c>
+      <c r="D181" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" t="s">
+        <v>97</v>
+      </c>
+      <c r="B182">
+        <v>2</v>
+      </c>
+      <c r="C182" t="s">
+        <v>15</v>
+      </c>
+      <c r="D182" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" t="s">
+        <v>62</v>
+      </c>
+      <c r="B183">
+        <v>300</v>
+      </c>
+      <c r="C183" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" t="s">
+        <v>133</v>
+      </c>
+      <c r="B184">
+        <v>2</v>
+      </c>
+      <c r="C184" t="s">
+        <v>15</v>
+      </c>
+      <c r="D184" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" t="s">
+        <v>108</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>15</v>
+      </c>
+      <c r="D185" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" t="s">
+        <v>141</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+      <c r="C186" t="s">
+        <v>15</v>
+      </c>
+      <c r="D186" s="2">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" t="s">
+        <v>142</v>
+      </c>
+      <c r="B187">
+        <v>2</v>
+      </c>
+      <c r="C187" t="s">
+        <v>15</v>
+      </c>
+      <c r="D187" s="2">
+        <v>45810</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added grocery list 9-6 , new ingredients, new recipes(BBQ)
</commit_message>
<xml_diff>
--- a/Excel_files/Log/Grocery_List_Log.xlsx
+++ b/Excel_files/Log/Grocery_List_Log.xlsx
@@ -8,20 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elskn\Projects\Grocery_list\Excel_files\Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AD2461-6270-42C4-A20A-55CE7FA0FA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C0B60B-A217-4016-A1FD-48A3B32B866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="504" windowWidth="12498" windowHeight="11802" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="396" windowWidth="11442" windowHeight="10680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log Per Recipe" sheetId="1" r:id="rId1"/>
     <sheet name="Log Combined" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="AvailableIngredients">[1]Ingredients!$A$2:$A$85</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="178">
   <si>
     <t>Recipe</t>
   </si>
@@ -450,13 +456,118 @@
   </si>
   <si>
     <t>Peer</t>
+  </si>
+  <si>
+    <t>BBQPORTOBELLOMETPERZIK</t>
+  </si>
+  <si>
+    <t>Portobello</t>
+  </si>
+  <si>
+    <t>PORTOBELLO</t>
+  </si>
+  <si>
+    <t>Geitenkaas</t>
+  </si>
+  <si>
+    <t>GEITENKAAS</t>
+  </si>
+  <si>
+    <t>Honing</t>
+  </si>
+  <si>
+    <t>HONING</t>
+  </si>
+  <si>
+    <t>Perzik blik</t>
+  </si>
+  <si>
+    <t>PERZIKBLIK</t>
+  </si>
+  <si>
+    <t>Noten</t>
+  </si>
+  <si>
+    <t>NOTEN</t>
+  </si>
+  <si>
+    <t>BBQMAÏSKOLVENMETMISOBIESLOOK</t>
+  </si>
+  <si>
+    <t>Maïskolf</t>
+  </si>
+  <si>
+    <t>MAÏSKOLF</t>
+  </si>
+  <si>
+    <t>Bieslook</t>
+  </si>
+  <si>
+    <t>BIESLOOK</t>
+  </si>
+  <si>
+    <t>Boter</t>
+  </si>
+  <si>
+    <t>BOTER</t>
+  </si>
+  <si>
+    <t>VEGGIEBURGERSMETKOMKOMMERSALADE</t>
+  </si>
+  <si>
+    <t>Veggieburger</t>
+  </si>
+  <si>
+    <t>VEGGIEBURGER</t>
+  </si>
+  <si>
+    <t>Hamburgerbroodje</t>
+  </si>
+  <si>
+    <t>HAMBURGERBROODJE</t>
+  </si>
+  <si>
+    <t>Mayonaise</t>
+  </si>
+  <si>
+    <t>MAYONAISE</t>
+  </si>
+  <si>
+    <t>Citroensap</t>
+  </si>
+  <si>
+    <t>CITROENSAP</t>
+  </si>
+  <si>
+    <t>Komkommer</t>
+  </si>
+  <si>
+    <t>KOMKOMMER</t>
+  </si>
+  <si>
+    <t>Lookpoeder</t>
+  </si>
+  <si>
+    <t>LOOKPOEDER</t>
+  </si>
+  <si>
+    <t>Mozarella sneetjes</t>
+  </si>
+  <si>
+    <t>MOZARELLASNEEJTES</t>
+  </si>
+  <si>
+    <t>Olijfolie</t>
+  </si>
+  <si>
+    <t>Smeerboter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +582,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,12 +628,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -532,6 +651,445 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Recipes"/>
+      <sheetName val="Ingredients"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Aardbei</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Ananas</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Anjovis</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Appel</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Aubergine</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Avocado</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Baguette</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Bakpoeder</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Banaan</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Bieslook</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Bladerdeeg</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Boter</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Broccoli</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Cavatappi</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Champignons</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Citroensap</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Courgette</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Druiven</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Edamame</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Ei</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Feta</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Geitenkaas</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>Gele Kiwi</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Granaatappel</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>Griekse Yoghurt</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>Hamburgerbroodje</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Honing</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Italiaanse Kruiden</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Kalamon Olijven</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>Kerstomaten</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>Ketchup</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Knoflookteen</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Komkommer</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Lenteui</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>Limoensap</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>Lookpoeder</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Maïs Klein Blik</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Maïskolf</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Mandarijn</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>Mayonaise</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>Melk</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>Mirin</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>Miso</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>Mosterd</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>Mozarella</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>Mozarella sneetjes</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>Noten</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>Olijfolie</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>Oregano</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>Passata</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>Peer</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>Perzik blik</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>Pindakaas</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>Pizzadeeg</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>Portobello</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>Prei</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>Proteïne Poeder</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>Rijst</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>Rijstazijn</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>Rode paprika</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>Rode Ui</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>Rode Wijnazijn</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>Scampi</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>Seitan</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>Skyr</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>Smeerboter</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>Soya melk</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>Soyasaus</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>Spaghetti</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>Spaghetti saus</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>Spitskool</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>Suiker</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>Super Gehakt</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>Tofu</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>Tomaat</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Vanille-extract</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>Vegan Yoghurt</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>Veggieburger</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>Volle Room</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>Wortel</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>Wrap</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>Yoghurt Esh</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>Zalm</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>Zout</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -819,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="G197" sqref="G197"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="G201" sqref="G201:G241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5431,17 +5989,968 @@
         <v>45810</v>
       </c>
     </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" t="s">
+        <v>57</v>
+      </c>
+      <c r="B201">
+        <v>12</v>
+      </c>
+      <c r="C201" t="s">
+        <v>58</v>
+      </c>
+      <c r="D201" t="s">
+        <v>59</v>
+      </c>
+      <c r="E201">
+        <v>2</v>
+      </c>
+      <c r="F201" t="s">
+        <v>15</v>
+      </c>
+      <c r="G201" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" t="s">
+        <v>57</v>
+      </c>
+      <c r="B202">
+        <v>12</v>
+      </c>
+      <c r="C202" t="s">
+        <v>60</v>
+      </c>
+      <c r="D202" t="s">
+        <v>61</v>
+      </c>
+      <c r="E202">
+        <v>468</v>
+      </c>
+      <c r="F202" t="s">
+        <v>10</v>
+      </c>
+      <c r="G202" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" t="s">
+        <v>57</v>
+      </c>
+      <c r="B203">
+        <v>12</v>
+      </c>
+      <c r="C203" t="s">
+        <v>62</v>
+      </c>
+      <c r="D203" t="s">
+        <v>63</v>
+      </c>
+      <c r="E203">
+        <v>300</v>
+      </c>
+      <c r="F203" t="s">
+        <v>10</v>
+      </c>
+      <c r="G203" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" t="s">
+        <v>57</v>
+      </c>
+      <c r="B204">
+        <v>12</v>
+      </c>
+      <c r="C204" t="s">
+        <v>64</v>
+      </c>
+      <c r="D204" t="s">
+        <v>65</v>
+      </c>
+      <c r="E204">
+        <v>180</v>
+      </c>
+      <c r="F204" t="s">
+        <v>10</v>
+      </c>
+      <c r="G204" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" t="s">
+        <v>57</v>
+      </c>
+      <c r="B205">
+        <v>12</v>
+      </c>
+      <c r="C205" t="s">
+        <v>53</v>
+      </c>
+      <c r="D205" t="s">
+        <v>54</v>
+      </c>
+      <c r="E205">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="F205" t="s">
+        <v>15</v>
+      </c>
+      <c r="G205" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" t="s">
+        <v>57</v>
+      </c>
+      <c r="B206">
+        <v>12</v>
+      </c>
+      <c r="C206" t="s">
+        <v>35</v>
+      </c>
+      <c r="D206" t="s">
+        <v>36</v>
+      </c>
+      <c r="E206">
+        <v>300</v>
+      </c>
+      <c r="F206" t="s">
+        <v>10</v>
+      </c>
+      <c r="G206" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" t="s">
+        <v>57</v>
+      </c>
+      <c r="B207">
+        <v>12</v>
+      </c>
+      <c r="C207" t="s">
+        <v>66</v>
+      </c>
+      <c r="D207" t="s">
+        <v>67</v>
+      </c>
+      <c r="E207">
+        <v>180</v>
+      </c>
+      <c r="F207" t="s">
+        <v>10</v>
+      </c>
+      <c r="G207" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" t="s">
+        <v>57</v>
+      </c>
+      <c r="B208">
+        <v>12</v>
+      </c>
+      <c r="C208" t="s">
+        <v>68</v>
+      </c>
+      <c r="D208" t="s">
+        <v>69</v>
+      </c>
+      <c r="E208">
+        <v>600</v>
+      </c>
+      <c r="F208" t="s">
+        <v>10</v>
+      </c>
+      <c r="G208" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" t="s">
+        <v>89</v>
+      </c>
+      <c r="B209">
+        <v>4</v>
+      </c>
+      <c r="C209" t="s">
+        <v>90</v>
+      </c>
+      <c r="D209" t="s">
+        <v>91</v>
+      </c>
+      <c r="E209">
+        <v>400</v>
+      </c>
+      <c r="F209" t="s">
+        <v>10</v>
+      </c>
+      <c r="G209" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" t="s">
+        <v>89</v>
+      </c>
+      <c r="B210">
+        <v>4</v>
+      </c>
+      <c r="C210" t="s">
+        <v>92</v>
+      </c>
+      <c r="D210" t="s">
+        <v>93</v>
+      </c>
+      <c r="E210">
+        <v>640</v>
+      </c>
+      <c r="F210" t="s">
+        <v>10</v>
+      </c>
+      <c r="G210" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" t="s">
+        <v>89</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="C211" t="s">
+        <v>64</v>
+      </c>
+      <c r="D211" t="s">
+        <v>65</v>
+      </c>
+      <c r="E211">
+        <v>200</v>
+      </c>
+      <c r="F211" t="s">
+        <v>10</v>
+      </c>
+      <c r="G211" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" t="s">
+        <v>89</v>
+      </c>
+      <c r="B212">
+        <v>4</v>
+      </c>
+      <c r="C212" t="s">
+        <v>68</v>
+      </c>
+      <c r="D212" t="s">
+        <v>69</v>
+      </c>
+      <c r="E212">
+        <v>180</v>
+      </c>
+      <c r="F212" t="s">
+        <v>10</v>
+      </c>
+      <c r="G212" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" t="s">
+        <v>81</v>
+      </c>
+      <c r="B213">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s">
+        <v>82</v>
+      </c>
+      <c r="D213" t="s">
+        <v>83</v>
+      </c>
+      <c r="E213">
+        <v>1</v>
+      </c>
+      <c r="F213" t="s">
+        <v>15</v>
+      </c>
+      <c r="G213" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" t="s">
+        <v>81</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+      <c r="C214" t="s">
+        <v>84</v>
+      </c>
+      <c r="D214" t="s">
+        <v>85</v>
+      </c>
+      <c r="E214">
+        <v>75</v>
+      </c>
+      <c r="F214" t="s">
+        <v>10</v>
+      </c>
+      <c r="G214" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" t="s">
+        <v>81</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+      <c r="C215" t="s">
+        <v>64</v>
+      </c>
+      <c r="D215" t="s">
+        <v>65</v>
+      </c>
+      <c r="E215">
+        <v>50</v>
+      </c>
+      <c r="F215" t="s">
+        <v>10</v>
+      </c>
+      <c r="G215" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" t="s">
+        <v>86</v>
+      </c>
+      <c r="B216">
+        <v>2</v>
+      </c>
+      <c r="C216" t="s">
+        <v>82</v>
+      </c>
+      <c r="D216" t="s">
+        <v>83</v>
+      </c>
+      <c r="E216">
+        <v>2</v>
+      </c>
+      <c r="F216" t="s">
+        <v>15</v>
+      </c>
+      <c r="G216" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" t="s">
+        <v>86</v>
+      </c>
+      <c r="B217">
+        <v>2</v>
+      </c>
+      <c r="C217" t="s">
+        <v>84</v>
+      </c>
+      <c r="D217" t="s">
+        <v>85</v>
+      </c>
+      <c r="E217">
+        <v>150</v>
+      </c>
+      <c r="F217" t="s">
+        <v>10</v>
+      </c>
+      <c r="G217" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" t="s">
+        <v>86</v>
+      </c>
+      <c r="B218">
+        <v>2</v>
+      </c>
+      <c r="C218" t="s">
+        <v>64</v>
+      </c>
+      <c r="D218" t="s">
+        <v>65</v>
+      </c>
+      <c r="E218">
+        <v>100</v>
+      </c>
+      <c r="F218" t="s">
+        <v>10</v>
+      </c>
+      <c r="G218" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" t="s">
+        <v>86</v>
+      </c>
+      <c r="B219">
+        <v>2</v>
+      </c>
+      <c r="C219" t="s">
+        <v>87</v>
+      </c>
+      <c r="D219" t="s">
+        <v>88</v>
+      </c>
+      <c r="E219">
+        <v>50</v>
+      </c>
+      <c r="F219" t="s">
+        <v>10</v>
+      </c>
+      <c r="G219" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" t="s">
+        <v>86</v>
+      </c>
+      <c r="B220">
+        <v>2</v>
+      </c>
+      <c r="C220" t="s">
+        <v>24</v>
+      </c>
+      <c r="D220" t="s">
+        <v>25</v>
+      </c>
+      <c r="E220">
+        <v>2</v>
+      </c>
+      <c r="F220" t="s">
+        <v>15</v>
+      </c>
+      <c r="G220" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" t="s">
+        <v>86</v>
+      </c>
+      <c r="B221">
+        <v>2</v>
+      </c>
+      <c r="C221" t="s">
+        <v>37</v>
+      </c>
+      <c r="D221" t="s">
+        <v>38</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+      <c r="F221" t="s">
+        <v>15</v>
+      </c>
+      <c r="G221" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" t="s">
+        <v>143</v>
+      </c>
+      <c r="B222">
+        <v>3</v>
+      </c>
+      <c r="C222" t="s">
+        <v>144</v>
+      </c>
+      <c r="D222" t="s">
+        <v>145</v>
+      </c>
+      <c r="E222" s="3">
+        <v>3</v>
+      </c>
+      <c r="F222" t="s">
+        <v>15</v>
+      </c>
+      <c r="G222" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223" t="s">
+        <v>143</v>
+      </c>
+      <c r="B223">
+        <v>3</v>
+      </c>
+      <c r="C223" t="s">
+        <v>146</v>
+      </c>
+      <c r="D223" t="s">
+        <v>147</v>
+      </c>
+      <c r="E223" s="3">
+        <v>150</v>
+      </c>
+      <c r="F223" t="s">
+        <v>10</v>
+      </c>
+      <c r="G223" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" t="s">
+        <v>143</v>
+      </c>
+      <c r="B224">
+        <v>3</v>
+      </c>
+      <c r="C224" t="s">
+        <v>148</v>
+      </c>
+      <c r="D224" t="s">
+        <v>149</v>
+      </c>
+      <c r="E224" s="3">
+        <v>30</v>
+      </c>
+      <c r="F224" t="s">
+        <v>10</v>
+      </c>
+      <c r="G224" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" t="s">
+        <v>143</v>
+      </c>
+      <c r="B225">
+        <v>3</v>
+      </c>
+      <c r="C225" t="s">
+        <v>150</v>
+      </c>
+      <c r="D225" t="s">
+        <v>151</v>
+      </c>
+      <c r="E225" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F225" t="s">
+        <v>15</v>
+      </c>
+      <c r="G225" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" t="s">
+        <v>143</v>
+      </c>
+      <c r="B226">
+        <v>3</v>
+      </c>
+      <c r="C226" t="s">
+        <v>152</v>
+      </c>
+      <c r="D226" t="s">
+        <v>153</v>
+      </c>
+      <c r="E226" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="F226" t="s">
+        <v>10</v>
+      </c>
+      <c r="G226" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" t="s">
+        <v>154</v>
+      </c>
+      <c r="B227">
+        <v>4</v>
+      </c>
+      <c r="C227" t="s">
+        <v>155</v>
+      </c>
+      <c r="D227" t="s">
+        <v>156</v>
+      </c>
+      <c r="E227" s="3">
+        <v>4</v>
+      </c>
+      <c r="F227" t="s">
+        <v>15</v>
+      </c>
+      <c r="G227" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228" t="s">
+        <v>154</v>
+      </c>
+      <c r="B228">
+        <v>4</v>
+      </c>
+      <c r="C228" t="s">
+        <v>66</v>
+      </c>
+      <c r="D228" t="s">
+        <v>67</v>
+      </c>
+      <c r="E228" s="3">
+        <v>75</v>
+      </c>
+      <c r="F228" t="s">
+        <v>10</v>
+      </c>
+      <c r="G228" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229" t="s">
+        <v>154</v>
+      </c>
+      <c r="B229">
+        <v>4</v>
+      </c>
+      <c r="C229" t="s">
+        <v>157</v>
+      </c>
+      <c r="D229" t="s">
+        <v>158</v>
+      </c>
+      <c r="E229" s="3">
+        <v>15</v>
+      </c>
+      <c r="F229" t="s">
+        <v>10</v>
+      </c>
+      <c r="G229" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A230" t="s">
+        <v>154</v>
+      </c>
+      <c r="B230">
+        <v>4</v>
+      </c>
+      <c r="C230" t="s">
+        <v>159</v>
+      </c>
+      <c r="D230" t="s">
+        <v>160</v>
+      </c>
+      <c r="E230" s="3">
+        <v>200</v>
+      </c>
+      <c r="F230" t="s">
+        <v>10</v>
+      </c>
+      <c r="G230" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A231" t="s">
+        <v>161</v>
+      </c>
+      <c r="B231">
+        <v>4</v>
+      </c>
+      <c r="C231" t="s">
+        <v>162</v>
+      </c>
+      <c r="D231" t="s">
+        <v>163</v>
+      </c>
+      <c r="E231" s="3">
+        <v>4</v>
+      </c>
+      <c r="F231" t="s">
+        <v>15</v>
+      </c>
+      <c r="G231" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A232" t="s">
+        <v>161</v>
+      </c>
+      <c r="B232">
+        <v>4</v>
+      </c>
+      <c r="C232" t="s">
+        <v>164</v>
+      </c>
+      <c r="D232" t="s">
+        <v>165</v>
+      </c>
+      <c r="E232" s="3">
+        <v>4</v>
+      </c>
+      <c r="F232" t="s">
+        <v>15</v>
+      </c>
+      <c r="G232" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A233" t="s">
+        <v>161</v>
+      </c>
+      <c r="B233">
+        <v>4</v>
+      </c>
+      <c r="C233" t="s">
+        <v>105</v>
+      </c>
+      <c r="D233" t="s">
+        <v>128</v>
+      </c>
+      <c r="E233" s="3">
+        <v>200</v>
+      </c>
+      <c r="F233" t="s">
+        <v>10</v>
+      </c>
+      <c r="G233" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A234" t="s">
+        <v>161</v>
+      </c>
+      <c r="B234">
+        <v>4</v>
+      </c>
+      <c r="C234" t="s">
+        <v>166</v>
+      </c>
+      <c r="D234" t="s">
+        <v>167</v>
+      </c>
+      <c r="E234" s="3">
+        <v>60</v>
+      </c>
+      <c r="F234" t="s">
+        <v>10</v>
+      </c>
+      <c r="G234" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A235" t="s">
+        <v>161</v>
+      </c>
+      <c r="B235">
+        <v>4</v>
+      </c>
+      <c r="C235" t="s">
+        <v>168</v>
+      </c>
+      <c r="D235" t="s">
+        <v>169</v>
+      </c>
+      <c r="E235" s="3">
+        <v>60</v>
+      </c>
+      <c r="F235" t="s">
+        <v>10</v>
+      </c>
+      <c r="G235" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A236" t="s">
+        <v>161</v>
+      </c>
+      <c r="B236">
+        <v>4</v>
+      </c>
+      <c r="C236" t="s">
+        <v>170</v>
+      </c>
+      <c r="D236" t="s">
+        <v>171</v>
+      </c>
+      <c r="E236" s="3">
+        <v>1</v>
+      </c>
+      <c r="F236" t="s">
+        <v>15</v>
+      </c>
+      <c r="G236" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237" t="s">
+        <v>161</v>
+      </c>
+      <c r="B237">
+        <v>4</v>
+      </c>
+      <c r="C237" t="s">
+        <v>157</v>
+      </c>
+      <c r="D237" t="s">
+        <v>158</v>
+      </c>
+      <c r="E237" s="3">
+        <v>60</v>
+      </c>
+      <c r="F237" t="s">
+        <v>10</v>
+      </c>
+      <c r="G237" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238" t="s">
+        <v>161</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+      <c r="C238" t="s">
+        <v>172</v>
+      </c>
+      <c r="D238" t="s">
+        <v>173</v>
+      </c>
+      <c r="E238" s="3">
+        <v>20</v>
+      </c>
+      <c r="F238" t="s">
+        <v>10</v>
+      </c>
+      <c r="G238" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239" t="s">
+        <v>161</v>
+      </c>
+      <c r="B239">
+        <v>4</v>
+      </c>
+      <c r="C239" t="s">
+        <v>32</v>
+      </c>
+      <c r="D239" t="s">
+        <v>33</v>
+      </c>
+      <c r="E239" s="3">
+        <v>4</v>
+      </c>
+      <c r="F239" t="s">
+        <v>15</v>
+      </c>
+      <c r="G239" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A240" t="s">
+        <v>161</v>
+      </c>
+      <c r="B240">
+        <v>4</v>
+      </c>
+      <c r="C240" t="s">
+        <v>110</v>
+      </c>
+      <c r="D240" t="s">
+        <v>117</v>
+      </c>
+      <c r="E240" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="F240" t="s">
+        <v>15</v>
+      </c>
+      <c r="G240" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241" t="s">
+        <v>161</v>
+      </c>
+      <c r="B241">
+        <v>4</v>
+      </c>
+      <c r="C241" t="s">
+        <v>174</v>
+      </c>
+      <c r="D241" t="s">
+        <v>175</v>
+      </c>
+      <c r="E241" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="F241" t="s">
+        <v>15</v>
+      </c>
+      <c r="G241" s="2">
+        <v>45817</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C222:C226" xr:uid="{1356703D-6423-46C9-8359-D7F6FCEC7294}">
+      <formula1>AvailableIngredients</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F222:F226" xr:uid="{B642A67C-13EE-4BD6-BFD6-8F9A028409BF}">
+      <formula1>"u,g"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D187"/>
+  <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="F223" sqref="F223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8068,6 +9577,566 @@
         <v>45810</v>
       </c>
     </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B188" s="4">
+        <v>1</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D188" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B189" s="4">
+        <v>50</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D189" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B190" s="4">
+        <v>18</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D190" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B191" s="4">
+        <v>1</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D191" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B192" s="4">
+        <v>2</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D192" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B193" s="4">
+        <v>300</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D193" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B194" s="4">
+        <v>1</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D194" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B195" s="4">
+        <v>2</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D195" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B196" s="4">
+        <v>1350</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D196" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B197" s="4">
+        <v>45.6</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D197" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B198" s="4">
+        <v>4</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D198" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B199" s="4">
+        <v>180</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D199" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B200" s="4">
+        <v>530</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D200" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B201" s="4">
+        <v>225</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D201" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B202" s="4">
+        <v>3</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D202" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B203" s="4">
+        <v>468</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D203" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B204" s="4">
+        <v>2</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D204" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B205" s="4">
+        <v>780</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D205" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B206" s="4">
+        <v>4</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D206" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B207" s="4">
+        <v>4</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D207" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B208" s="4">
+        <v>400</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B209" s="4">
+        <v>640</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D209" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B210" s="4">
+        <v>2</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D210" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B211" s="4">
+        <v>300</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D211" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B212" s="4">
+        <v>1</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D212" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B213" s="4">
+        <v>1</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D213" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B214" s="4">
+        <v>3</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D214" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B215" s="4">
+        <v>1</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D215" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B216" s="4">
+        <v>1</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D216" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B217" s="4">
+        <v>4</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D217" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B218" s="4">
+        <v>30</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D218" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B219" s="4">
+        <v>200</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D219" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B220" s="4">
+        <v>4</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D220" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B221" s="4">
+        <v>4</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D221" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B222" s="4">
+        <v>1</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D222" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B223" s="4">
+        <v>3</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D223" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B224" s="4">
+        <v>1</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D224" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B225" s="4">
+        <v>1</v>
+      </c>
+      <c r="C225" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D225" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B226" s="4">
+        <v>1</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D226" s="2">
+        <v>45817</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B227" s="4">
+        <v>2</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D227" s="2">
+        <v>45817</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>